<commit_message>
Updated return statistics + new scenario generation method
</commit_message>
<xml_diff>
--- a/Data/Forecasts/DA/2023-12-01_exo[].xlsx
+++ b/Data/Forecasts/DA/2023-12-01_exo[].xlsx
@@ -454,7 +454,7 @@
         <v>45261</v>
       </c>
       <c r="B2" t="n">
-        <v>113.307991027832</v>
+        <v>106.197998046875</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         <v>45261.02083333334</v>
       </c>
       <c r="B3" t="n">
-        <v>113.129264831543</v>
+        <v>106.1641540527344</v>
       </c>
     </row>
     <row r="4">
@@ -470,7 +470,7 @@
         <v>45261.04166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>110.8886489868164</v>
+        <v>106.2518692016602</v>
       </c>
     </row>
     <row r="5">
@@ -478,7 +478,7 @@
         <v>45261.0625</v>
       </c>
       <c r="B5" t="n">
-        <v>110.6936569213867</v>
+        <v>106.2052459716797</v>
       </c>
     </row>
     <row r="6">
@@ -486,7 +486,7 @@
         <v>45261.08333333334</v>
       </c>
       <c r="B6" t="n">
-        <v>108.7412567138672</v>
+        <v>104.5456314086914</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         <v>45261.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>108.6662750244141</v>
+        <v>104.4966812133789</v>
       </c>
     </row>
     <row r="8">
@@ -502,7 +502,7 @@
         <v>45261.125</v>
       </c>
       <c r="B8" t="n">
-        <v>106.9172821044922</v>
+        <v>103.8380813598633</v>
       </c>
     </row>
     <row r="9">
@@ -510,7 +510,7 @@
         <v>45261.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>106.7928314208984</v>
+        <v>103.7358627319336</v>
       </c>
     </row>
     <row r="10">
@@ -518,7 +518,7 @@
         <v>45261.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>106.6519927978516</v>
+        <v>104.6287536621094</v>
       </c>
     </row>
     <row r="11">
@@ -526,7 +526,7 @@
         <v>45261.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>106.5378723144531</v>
+        <v>104.5373153686523</v>
       </c>
     </row>
     <row r="12">
@@ -534,7 +534,7 @@
         <v>45261.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>109.7129364013672</v>
+        <v>109.8541107177734</v>
       </c>
     </row>
     <row r="13">
@@ -542,7 +542,7 @@
         <v>45261.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>109.6101455688477</v>
+        <v>109.7744293212891</v>
       </c>
     </row>
     <row r="14">
@@ -550,7 +550,7 @@
         <v>45261.25</v>
       </c>
       <c r="B14" t="n">
-        <v>120.5264205932617</v>
+        <v>123.1528549194336</v>
       </c>
     </row>
     <row r="15">
@@ -558,7 +558,7 @@
         <v>45261.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>120.434326171875</v>
+        <v>123.0840606689453</v>
       </c>
     </row>
     <row r="16">
@@ -566,7 +566,7 @@
         <v>45261.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>143.1932067871094</v>
+        <v>140.2832336425781</v>
       </c>
     </row>
     <row r="17">
@@ -574,7 +574,7 @@
         <v>45261.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>143.1109161376953</v>
+        <v>140.2240447998047</v>
       </c>
     </row>
     <row r="18">
@@ -582,7 +582,7 @@
         <v>45261.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>161.6958312988281</v>
+        <v>151.8777313232422</v>
       </c>
     </row>
     <row r="19">
@@ -590,7 +590,7 @@
         <v>45261.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>161.6235656738281</v>
+        <v>151.8302764892578</v>
       </c>
     </row>
     <row r="20">
@@ -598,7 +598,7 @@
         <v>45261.375</v>
       </c>
       <c r="B20" t="n">
-        <v>180.0274353027344</v>
+        <v>162.6111602783203</v>
       </c>
     </row>
     <row r="21">
@@ -606,7 +606,7 @@
         <v>45261.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>179.9600219726562</v>
+        <v>162.5661926269531</v>
       </c>
     </row>
     <row r="22">
@@ -614,7 +614,7 @@
         <v>45261.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>179.105224609375</v>
+        <v>162.53466796875</v>
       </c>
     </row>
     <row r="23">
@@ -622,7 +622,7 @@
         <v>45261.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>179.0423126220703</v>
+        <v>162.4917144775391</v>
       </c>
     </row>
     <row r="24">
@@ -630,7 +630,7 @@
         <v>45261.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>167.639892578125</v>
+        <v>156.7200622558594</v>
       </c>
     </row>
     <row r="25">
@@ -638,7 +638,7 @@
         <v>45261.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>167.5807342529297</v>
+        <v>156.6782531738281</v>
       </c>
     </row>
     <row r="26">
@@ -646,7 +646,7 @@
         <v>45261.5</v>
       </c>
       <c r="B26" t="n">
-        <v>169.1214904785156</v>
+        <v>159.3792266845703</v>
       </c>
     </row>
     <row r="27">
@@ -654,7 +654,7 @@
         <v>45261.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>169.0651092529297</v>
+        <v>159.3375854492188</v>
       </c>
     </row>
     <row r="28">
@@ -662,7 +662,7 @@
         <v>45261.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>161.09716796875</v>
+        <v>154.4311981201172</v>
       </c>
     </row>
     <row r="29">
@@ -670,7 +670,7 @@
         <v>45261.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>161.0423278808594</v>
+        <v>154.3886871337891</v>
       </c>
     </row>
     <row r="30">
@@ -678,7 +678,7 @@
         <v>45261.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>158.1585693359375</v>
+        <v>155.5289001464844</v>
       </c>
     </row>
     <row r="31">
@@ -686,7 +686,7 @@
         <v>45261.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>158.1042327880859</v>
+        <v>155.4848327636719</v>
       </c>
     </row>
     <row r="32">
@@ -694,7 +694,7 @@
         <v>45261.625</v>
       </c>
       <c r="B32" t="n">
-        <v>170.0274810791016</v>
+        <v>164.8945922851562</v>
       </c>
     </row>
     <row r="33">
@@ -702,7 +702,7 @@
         <v>45261.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>169.9727325439453</v>
+        <v>164.8486328125</v>
       </c>
     </row>
     <row r="34">
@@ -710,7 +710,7 @@
         <v>45261.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>187.93408203125</v>
+        <v>187.7915954589844</v>
       </c>
     </row>
     <row r="35">
@@ -718,7 +718,7 @@
         <v>45261.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>187.8776245117188</v>
+        <v>187.7430725097656</v>
       </c>
     </row>
     <row r="36">
@@ -726,7 +726,7 @@
         <v>45261.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>213.3716125488281</v>
+        <v>211.5</v>
       </c>
     </row>
     <row r="37">
@@ -734,7 +734,7 @@
         <v>45261.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>213.3119964599609</v>
+        <v>211.4480743408203</v>
       </c>
     </row>
     <row r="38">
@@ -742,7 +742,7 @@
         <v>45261.75</v>
       </c>
       <c r="B38" t="n">
-        <v>189.0390014648438</v>
+        <v>186.4666290283203</v>
       </c>
     </row>
     <row r="39">
@@ -750,7 +750,7 @@
         <v>45261.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>188.9747314453125</v>
+        <v>186.4101715087891</v>
       </c>
     </row>
     <row r="40">
@@ -758,7 +758,7 @@
         <v>45261.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>167.2014617919922</v>
+        <v>163.5970153808594</v>
       </c>
     </row>
     <row r="41">
@@ -766,7 +766,7 @@
         <v>45261.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>167.1309356689453</v>
+        <v>163.5346374511719</v>
       </c>
     </row>
     <row r="42">
@@ -774,7 +774,7 @@
         <v>45261.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>150.0362854003906</v>
+        <v>147.7666931152344</v>
       </c>
     </row>
     <row r="43">
@@ -782,7 +782,7 @@
         <v>45261.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>149.9581298828125</v>
+        <v>147.697021484375</v>
       </c>
     </row>
     <row r="44">
@@ -790,7 +790,7 @@
         <v>45261.875</v>
       </c>
       <c r="B44" t="n">
-        <v>132.8030548095703</v>
+        <v>136.4794616699219</v>
       </c>
     </row>
     <row r="45">
@@ -798,7 +798,7 @@
         <v>45261.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>132.7161102294922</v>
+        <v>136.4012603759766</v>
       </c>
     </row>
     <row r="46">
@@ -806,7 +806,7 @@
         <v>45261.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>129.1320648193359</v>
+        <v>125.8640823364258</v>
       </c>
     </row>
     <row r="47">
@@ -814,7 +814,7 @@
         <v>45261.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>129.0353546142578</v>
+        <v>125.7766876220703</v>
       </c>
     </row>
     <row r="48">
@@ -822,7 +822,7 @@
         <v>45261.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>115.6702041625977</v>
+        <v>124.4602890014648</v>
       </c>
     </row>
     <row r="49">
@@ -830,7 +830,7 @@
         <v>45261.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>115.5646209716797</v>
+        <v>124.3642807006836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>